<commit_message>
Remove rpart and add 50percent cutoff based on JKL feedback
</commit_message>
<xml_diff>
--- a/data/signature_results.xlsx
+++ b/data/signature_results.xlsx
@@ -3922,10 +3922,10 @@
         <v>-2.06307415916792</v>
       </c>
       <c r="C7" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4020,10 +4020,10 @@
         <v>-1.806268042965875</v>
       </c>
       <c r="C14" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -4034,10 +4034,10 @@
         <v>-1.620583148051273</v>
       </c>
       <c r="C15" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -4062,10 +4062,10 @@
         <v>-1.596314362819832</v>
       </c>
       <c r="C17" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -4090,10 +4090,10 @@
         <v>-1.574610177556519</v>
       </c>
       <c r="C19" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -4132,10 +4132,10 @@
         <v>-1.946730541836411</v>
       </c>
       <c r="C22" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -4146,10 +4146,10 @@
         <v>-1.687521288018933</v>
       </c>
       <c r="C23" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -4160,10 +4160,10 @@
         <v>-1.640728731465615</v>
       </c>
       <c r="C24" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -4244,10 +4244,10 @@
         <v>-1.840982873250805</v>
       </c>
       <c r="C30" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -4286,10 +4286,10 @@
         <v>-1.885733008767205</v>
       </c>
       <c r="C33" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -4342,10 +4342,10 @@
         <v>-1.743493047793878</v>
       </c>
       <c r="C37" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -4356,10 +4356,10 @@
         <v>-1.745824856911583</v>
       </c>
       <c r="C38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -4384,10 +4384,10 @@
         <v>-1.804091209132586</v>
       </c>
       <c r="C40" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -4398,10 +4398,10 @@
         <v>-1.655124288395738</v>
       </c>
       <c r="C41" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -4426,10 +4426,10 @@
         <v>-1.804856378801607</v>
       </c>
       <c r="C43" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -4482,10 +4482,10 @@
         <v>-1.990350711692934</v>
       </c>
       <c r="C47" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -4524,10 +4524,10 @@
         <v>-1.691859709866431</v>
       </c>
       <c r="C50" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -4650,10 +4650,10 @@
         <v>-1.86499242528775</v>
       </c>
       <c r="C59" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -4678,10 +4678,10 @@
         <v>-1.756120838938014</v>
       </c>
       <c r="C61" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -4692,10 +4692,10 @@
         <v>-1.696749594423806</v>
       </c>
       <c r="C62" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -4706,10 +4706,10 @@
         <v>-1.993856340183016</v>
       </c>
       <c r="C63" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -4734,10 +4734,10 @@
         <v>-1.938282042335604</v>
       </c>
       <c r="C65" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -4748,10 +4748,10 @@
         <v>-1.748615880242408</v>
       </c>
       <c r="C66" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -4776,10 +4776,10 @@
         <v>-1.86445403892693</v>
       </c>
       <c r="C68" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -4818,10 +4818,10 @@
         <v>-1.832598283017753</v>
       </c>
       <c r="C71" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -4860,10 +4860,10 @@
         <v>-1.91456497046877</v>
       </c>
       <c r="C74" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -4902,10 +4902,10 @@
         <v>-2.038709713107681</v>
       </c>
       <c r="C77" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D77">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -4972,10 +4972,10 @@
         <v>-1.851101250557012</v>
       </c>
       <c r="C82" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -5000,10 +5000,10 @@
         <v>-2.030088796976381</v>
       </c>
       <c r="C84" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D84">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -5154,10 +5154,10 @@
         <v>-1.722822868628791</v>
       </c>
       <c r="C95" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D95">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -5168,10 +5168,10 @@
         <v>-1.68794534982122</v>
       </c>
       <c r="C96" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D96">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -5238,10 +5238,10 @@
         <v>-1.535917176556776</v>
       </c>
       <c r="C101" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -5252,10 +5252,10 @@
         <v>-1.714023813379839</v>
       </c>
       <c r="C102" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D102">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -5280,10 +5280,10 @@
         <v>-1.873161539614415</v>
       </c>
       <c r="C104" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D104">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -5308,10 +5308,10 @@
         <v>-2.009162155625346</v>
       </c>
       <c r="C106" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D106">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -5392,10 +5392,10 @@
         <v>-1.992970310908802</v>
       </c>
       <c r="C112" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D112">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -5448,10 +5448,10 @@
         <v>-1.694504667525941</v>
       </c>
       <c r="C116" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D116">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -5490,10 +5490,10 @@
         <v>-1.602926740051456</v>
       </c>
       <c r="C119" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D119">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -5546,10 +5546,10 @@
         <v>-1.924309685100072</v>
       </c>
       <c r="C123" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D123">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -5616,10 +5616,10 @@
         <v>-1.633343841782809</v>
       </c>
       <c r="C128" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D128">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -5784,10 +5784,10 @@
         <v>-1.959368550217227</v>
       </c>
       <c r="C140" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D140">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -5798,10 +5798,10 @@
         <v>-1.969428853912699</v>
       </c>
       <c r="C141" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D141">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -5812,10 +5812,10 @@
         <v>-1.859180805145756</v>
       </c>
       <c r="C142" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D142">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -5854,10 +5854,10 @@
         <v>-1.662203661311719</v>
       </c>
       <c r="C145" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D145">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -5868,10 +5868,10 @@
         <v>-1.561415467790296</v>
       </c>
       <c r="C146" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D146">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -6036,10 +6036,10 @@
         <v>-1.580690377785164</v>
       </c>
       <c r="C158" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D158">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -6050,10 +6050,10 @@
         <v>-1.86256341155624</v>
       </c>
       <c r="C159" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D159">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -6064,10 +6064,10 @@
         <v>-1.678547103220077</v>
       </c>
       <c r="C160" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D160">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -6106,10 +6106,10 @@
         <v>-1.939176055629251</v>
       </c>
       <c r="C163" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D163">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -6134,10 +6134,10 @@
         <v>-2.023528451658239</v>
       </c>
       <c r="C165" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D165">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -6176,10 +6176,10 @@
         <v>-1.634140390747732</v>
       </c>
       <c r="C168" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D168">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -6190,10 +6190,10 @@
         <v>-1.658415838926596</v>
       </c>
       <c r="C169" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D169">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -6274,10 +6274,10 @@
         <v>-1.561797811563123</v>
       </c>
       <c r="C175" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D175">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -6288,10 +6288,10 @@
         <v>-1.819006560913885</v>
       </c>
       <c r="C176" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D176">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -6330,10 +6330,10 @@
         <v>-1.584794952621134</v>
       </c>
       <c r="C179" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D179">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -6484,10 +6484,10 @@
         <v>-1.777887868406314</v>
       </c>
       <c r="C190" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D190">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -6638,10 +6638,10 @@
         <v>-1.623134327394259</v>
       </c>
       <c r="C201" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D201">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="1:4">
@@ -6680,10 +6680,10 @@
         <v>-1.761923501780635</v>
       </c>
       <c r="C204" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D204">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -6736,10 +6736,10 @@
         <v>-1.873611515248272</v>
       </c>
       <c r="C208" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D208">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -6764,10 +6764,10 @@
         <v>-2.066948653527179</v>
       </c>
       <c r="C210" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D210">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -6792,10 +6792,10 @@
         <v>-1.801929473050743</v>
       </c>
       <c r="C212" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D212">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -6806,10 +6806,10 @@
         <v>-1.745412663024774</v>
       </c>
       <c r="C213" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D213">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -6834,10 +6834,10 @@
         <v>-1.765600741698591</v>
       </c>
       <c r="C215" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D215">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -6848,10 +6848,10 @@
         <v>-2.065686424856243</v>
       </c>
       <c r="C216" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D216">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -6960,10 +6960,10 @@
         <v>-1.762612719014886</v>
       </c>
       <c r="C224" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D224">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -6974,10 +6974,10 @@
         <v>-2.033830985595531</v>
       </c>
       <c r="C225" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D225">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -6988,10 +6988,10 @@
         <v>-1.731161219780125</v>
       </c>
       <c r="C226" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D226">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -7016,10 +7016,10 @@
         <v>-1.567147960721043</v>
       </c>
       <c r="C228" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D228">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -7128,10 +7128,10 @@
         <v>-1.534566212149355</v>
       </c>
       <c r="C236" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D236">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -7296,10 +7296,10 @@
         <v>-1.95921098769358</v>
       </c>
       <c r="C248" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D248">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="249" spans="1:4">
@@ -7324,10 +7324,10 @@
         <v>-1.694306424654629</v>
       </c>
       <c r="C250" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D250">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -7338,10 +7338,10 @@
         <v>-1.901039204301521</v>
       </c>
       <c r="C251" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D251">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -7394,10 +7394,10 @@
         <v>-1.852590089310582</v>
       </c>
       <c r="C255" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D255">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="256" spans="1:4">
@@ -7408,10 +7408,10 @@
         <v>-1.735251054199933</v>
       </c>
       <c r="C256" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D256">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="257" spans="1:4">
@@ -7422,10 +7422,10 @@
         <v>-1.838592373977753</v>
       </c>
       <c r="C257" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D257">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="258" spans="1:4">
@@ -7548,10 +7548,10 @@
         <v>-1.594660663009556</v>
       </c>
       <c r="C266" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D266">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="267" spans="1:4">
@@ -7562,10 +7562,10 @@
         <v>-2.037434349779434</v>
       </c>
       <c r="C267" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D267">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="268" spans="1:4">
@@ -7576,10 +7576,10 @@
         <v>-1.690035970968262</v>
       </c>
       <c r="C268" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D268">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="269" spans="1:4">
@@ -7632,10 +7632,10 @@
         <v>-1.912282606118101</v>
       </c>
       <c r="C272" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D272">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="273" spans="1:4">
@@ -7674,10 +7674,10 @@
         <v>-1.605561336551875</v>
       </c>
       <c r="C275" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D275">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -7688,10 +7688,10 @@
         <v>-1.67708568195856</v>
       </c>
       <c r="C276" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D276">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="277" spans="1:4">
@@ -7702,10 +7702,10 @@
         <v>-1.88254692097401</v>
       </c>
       <c r="C277" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D277">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="278" spans="1:4">
@@ -7744,10 +7744,10 @@
         <v>-1.756727833011233</v>
       </c>
       <c r="C280" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D280">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="281" spans="1:4">
@@ -7772,10 +7772,10 @@
         <v>-1.928587596461284</v>
       </c>
       <c r="C282" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D282">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="283" spans="1:4">
@@ -7800,10 +7800,10 @@
         <v>-1.723192085420213</v>
       </c>
       <c r="C284" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D284">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="285" spans="1:4">
@@ -7814,10 +7814,10 @@
         <v>-1.807001396469012</v>
       </c>
       <c r="C285" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D285">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="286" spans="1:4">
@@ -7828,10 +7828,10 @@
         <v>-1.558573353082008</v>
       </c>
       <c r="C286" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D286">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -7842,10 +7842,10 @@
         <v>-1.646933571993062</v>
       </c>
       <c r="C287" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D287">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="288" spans="1:4">
@@ -7856,10 +7856,10 @@
         <v>-1.79496386132225</v>
       </c>
       <c r="C288" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D288">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="289" spans="1:4">
@@ -7898,10 +7898,10 @@
         <v>-1.727183535455192</v>
       </c>
       <c r="C291" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D291">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="292" spans="1:4">
@@ -7982,10 +7982,10 @@
         <v>-1.752236388752778</v>
       </c>
       <c r="C297" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D297">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="298" spans="1:4">
@@ -7996,10 +7996,10 @@
         <v>-1.765367140571898</v>
       </c>
       <c r="C298" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D298">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="299" spans="1:4">
@@ -8010,10 +8010,10 @@
         <v>-1.960175323469497</v>
       </c>
       <c r="C299" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D299">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="300" spans="1:4">
@@ -8038,10 +8038,10 @@
         <v>-1.908949465275289</v>
       </c>
       <c r="C301" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D301">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="302" spans="1:4">
@@ -8080,10 +8080,10 @@
         <v>-1.944925729038921</v>
       </c>
       <c r="C304" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D304">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="305" spans="1:4">
@@ -8150,10 +8150,10 @@
         <v>-1.606341338329883</v>
       </c>
       <c r="C309" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D309">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="310" spans="1:4">
@@ -8220,10 +8220,10 @@
         <v>-1.755161152307182</v>
       </c>
       <c r="C314" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D314">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="315" spans="1:4">
@@ -8234,10 +8234,10 @@
         <v>-1.743294978911764</v>
       </c>
       <c r="C315" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D315">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="316" spans="1:4">
@@ -8248,10 +8248,10 @@
         <v>-1.89719255108088</v>
       </c>
       <c r="C316" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D316">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="317" spans="1:4">
@@ -8262,10 +8262,10 @@
         <v>-1.802456707439814</v>
       </c>
       <c r="C317" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D317">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="318" spans="1:4">
@@ -8374,10 +8374,10 @@
         <v>-1.60233252097254</v>
       </c>
       <c r="C325" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D325">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="326" spans="1:4">
@@ -8514,10 +8514,10 @@
         <v>-1.573824575840668</v>
       </c>
       <c r="C335" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D335">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="336" spans="1:4">
@@ -8528,10 +8528,10 @@
         <v>-1.742228968088872</v>
       </c>
       <c r="C336" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D336">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="337" spans="1:4">
@@ -8598,10 +8598,10 @@
         <v>-1.648344808304745</v>
       </c>
       <c r="C341" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D341">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="342" spans="1:4">
@@ -8654,10 +8654,10 @@
         <v>-1.739147844665597</v>
       </c>
       <c r="C345" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D345">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="346" spans="1:4">
@@ -8668,10 +8668,10 @@
         <v>-1.82057982452638</v>
       </c>
       <c r="C346" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D346">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="347" spans="1:4">
@@ -8738,10 +8738,10 @@
         <v>-2.019338253386453</v>
       </c>
       <c r="C351" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D351">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="352" spans="1:4">
@@ -8836,10 +8836,10 @@
         <v>-1.863624181620201</v>
       </c>
       <c r="C358" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D358">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="359" spans="1:4">
@@ -8850,10 +8850,10 @@
         <v>-1.857280304044075</v>
       </c>
       <c r="C359" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D359">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="360" spans="1:4">
@@ -8878,10 +8878,10 @@
         <v>-1.955479634570307</v>
       </c>
       <c r="C361" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D361">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="362" spans="1:4">
@@ -8920,10 +8920,10 @@
         <v>-1.589750457919949</v>
       </c>
       <c r="C364" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D364">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="365" spans="1:4">
@@ -8962,10 +8962,10 @@
         <v>-1.651822692331087</v>
       </c>
       <c r="C367" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D367">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="368" spans="1:4">
@@ -9088,10 +9088,10 @@
         <v>-1.696195265060944</v>
       </c>
       <c r="C376" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D376">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="377" spans="1:4">
@@ -9116,10 +9116,10 @@
         <v>-1.929323433170805</v>
       </c>
       <c r="C378" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D378">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="379" spans="1:4">
@@ -9172,10 +9172,10 @@
         <v>-1.773563610306497</v>
       </c>
       <c r="C382" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D382">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="383" spans="1:4">
@@ -9200,10 +9200,10 @@
         <v>-2.050046637747273</v>
       </c>
       <c r="C384" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D384">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="385" spans="1:4">
@@ -9256,10 +9256,10 @@
         <v>-1.728187148985576</v>
       </c>
       <c r="C388" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D388">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="389" spans="1:4">
@@ -9312,10 +9312,10 @@
         <v>-1.874768357708149</v>
       </c>
       <c r="C392" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D392">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="393" spans="1:4">
@@ -9326,10 +9326,10 @@
         <v>-1.732610635300398</v>
       </c>
       <c r="C393" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D393">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="394" spans="1:4">
@@ -9368,10 +9368,10 @@
         <v>-1.895696560062693</v>
       </c>
       <c r="C396" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D396">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="397" spans="1:4">
@@ -9382,10 +9382,10 @@
         <v>-1.54324025527494</v>
       </c>
       <c r="C397" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D397">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="398" spans="1:4">
@@ -9452,10 +9452,10 @@
         <v>-1.539328799022821</v>
       </c>
       <c r="C402" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D402">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="403" spans="1:4">
@@ -9536,10 +9536,10 @@
         <v>-1.614268447120501</v>
       </c>
       <c r="C408" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D408">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="409" spans="1:4">
@@ -9634,10 +9634,10 @@
         <v>-1.969444535987663</v>
       </c>
       <c r="C415" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D415">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="416" spans="1:4">
@@ -9732,10 +9732,10 @@
         <v>-1.766976078648375</v>
       </c>
       <c r="C422" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D422">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="423" spans="1:4">
@@ -9746,10 +9746,10 @@
         <v>-1.74262500378685</v>
       </c>
       <c r="C423" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D423">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="424" spans="1:4">
@@ -9760,10 +9760,10 @@
         <v>-1.901591116028857</v>
       </c>
       <c r="C424" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D424">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="425" spans="1:4">
@@ -9844,10 +9844,10 @@
         <v>-2.059471543225361</v>
       </c>
       <c r="C430" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D430">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="431" spans="1:4">
@@ -9942,10 +9942,10 @@
         <v>-1.701207252552385</v>
       </c>
       <c r="C437" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D437">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="438" spans="1:4">
@@ -9984,10 +9984,10 @@
         <v>-1.895837784550108</v>
       </c>
       <c r="C440" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D440">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="441" spans="1:4">
@@ -9998,10 +9998,10 @@
         <v>-1.662147400092239</v>
       </c>
       <c r="C441" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D441">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="442" spans="1:4">
@@ -10110,10 +10110,10 @@
         <v>-1.883560976740207</v>
       </c>
       <c r="C449" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D449">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="450" spans="1:4">
@@ -10264,10 +10264,10 @@
         <v>-1.903176693454962</v>
       </c>
       <c r="C460" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D460">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="461" spans="1:4">
@@ -10292,10 +10292,10 @@
         <v>-2.048703156433445</v>
       </c>
       <c r="C462" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D462">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="463" spans="1:4">
@@ -10418,10 +10418,10 @@
         <v>-1.8968015530276</v>
       </c>
       <c r="C471" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D471">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="472" spans="1:4">
@@ -10488,10 +10488,10 @@
         <v>-1.670281001234579</v>
       </c>
       <c r="C476" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D476">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="477" spans="1:4">
@@ -10544,10 +10544,10 @@
         <v>-1.729266694205009</v>
       </c>
       <c r="C480" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D480">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="481" spans="1:4">
@@ -10558,10 +10558,10 @@
         <v>-1.877442030056534</v>
       </c>
       <c r="C481" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D481">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="482" spans="1:4">
@@ -10586,10 +10586,10 @@
         <v>-1.749220533824453</v>
       </c>
       <c r="C483" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D483">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="484" spans="1:4">
@@ -10600,10 +10600,10 @@
         <v>-2.009721426651254</v>
       </c>
       <c r="C484" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D484">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="485" spans="1:4">
@@ -10614,10 +10614,10 @@
         <v>-1.769006353202528</v>
       </c>
       <c r="C485" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D485">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="486" spans="1:4">
@@ -10656,10 +10656,10 @@
         <v>-1.953540184621357</v>
       </c>
       <c r="C488" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D488">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="489" spans="1:4">
@@ -10698,10 +10698,10 @@
         <v>-2.024589140193247</v>
       </c>
       <c r="C491" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D491">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="492" spans="1:4">
@@ -10712,10 +10712,10 @@
         <v>-1.573380514492616</v>
       </c>
       <c r="C492" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D492">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="493" spans="1:4">
@@ -10726,10 +10726,10 @@
         <v>-1.560990956944726</v>
       </c>
       <c r="C493" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D493">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="494" spans="1:4">
@@ -10796,10 +10796,10 @@
         <v>-1.893431231417576</v>
       </c>
       <c r="C498" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D498">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="499" spans="1:4">
@@ -10810,10 +10810,10 @@
         <v>-1.57394141666939</v>
       </c>
       <c r="C499" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D499">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="500" spans="1:4">
@@ -10824,10 +10824,10 @@
         <v>-1.586959237725799</v>
       </c>
       <c r="C500" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D500">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="501" spans="1:4">
@@ -10852,10 +10852,10 @@
         <v>-1.844945646218207</v>
       </c>
       <c r="C502" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D502">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="503" spans="1:4">
@@ -10894,10 +10894,10 @@
         <v>-2.040525698996417</v>
       </c>
       <c r="C505" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D505">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="506" spans="1:4">
@@ -10936,10 +10936,10 @@
         <v>-1.623691165162289</v>
       </c>
       <c r="C508" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D508">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="509" spans="1:4">
@@ -10978,10 +10978,10 @@
         <v>-1.58067566490002</v>
       </c>
       <c r="C511" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D511">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="512" spans="1:4">
@@ -10992,10 +10992,10 @@
         <v>-2.040632135586947</v>
       </c>
       <c r="C512" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D512">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="513" spans="1:4">
@@ -11020,10 +11020,10 @@
         <v>-2.031457658783237</v>
       </c>
       <c r="C514" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D514">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="515" spans="1:4">
@@ -11034,10 +11034,10 @@
         <v>-1.790236761222223</v>
       </c>
       <c r="C515" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D515">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="516" spans="1:4">
@@ -11048,10 +11048,10 @@
         <v>-2.044399846939368</v>
       </c>
       <c r="C516" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D516">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="517" spans="1:4">
@@ -11118,10 +11118,10 @@
         <v>-1.940984532523147</v>
       </c>
       <c r="C521" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D521">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="522" spans="1:4">
@@ -11146,10 +11146,10 @@
         <v>-1.777373345241485</v>
       </c>
       <c r="C523" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D523">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="524" spans="1:4">
@@ -11188,10 +11188,10 @@
         <v>-1.806598769318281</v>
       </c>
       <c r="C526" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D526">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="527" spans="1:4">
@@ -11216,10 +11216,10 @@
         <v>-1.97295781256314</v>
       </c>
       <c r="C528" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D528">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="529" spans="1:4">
@@ -11230,10 +11230,10 @@
         <v>-1.989453868149982</v>
       </c>
       <c r="C529" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D529">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="530" spans="1:4">
@@ -11300,10 +11300,10 @@
         <v>-2.066528708416752</v>
       </c>
       <c r="C534" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D534">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="535" spans="1:4">
@@ -11356,10 +11356,10 @@
         <v>-1.935150643196155</v>
       </c>
       <c r="C538" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D538">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="539" spans="1:4">
@@ -11398,10 +11398,10 @@
         <v>-1.645361372854956</v>
       </c>
       <c r="C541" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D541">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="542" spans="1:4">
@@ -11440,10 +11440,10 @@
         <v>-1.652872347169891</v>
       </c>
       <c r="C544" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D544">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="545" spans="1:4">
@@ -11454,10 +11454,10 @@
         <v>-2.06287642400505</v>
       </c>
       <c r="C545" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D545">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="546" spans="1:4">
@@ -11524,10 +11524,10 @@
         <v>-2.062037826521802</v>
       </c>
       <c r="C550" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D550">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="551" spans="1:4">
@@ -11552,10 +11552,10 @@
         <v>-1.938232446962756</v>
       </c>
       <c r="C552" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D552">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="553" spans="1:4">
@@ -11566,10 +11566,10 @@
         <v>-1.88653180021508</v>
       </c>
       <c r="C553" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D553">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="554" spans="1:4">
@@ -11622,10 +11622,10 @@
         <v>-1.655190642611039</v>
       </c>
       <c r="C557" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D557">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="558" spans="1:4">
@@ -11734,10 +11734,10 @@
         <v>-1.906106014907668</v>
       </c>
       <c r="C565" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D565">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="566" spans="1:4">
@@ -11762,10 +11762,10 @@
         <v>-1.801524823903979</v>
       </c>
       <c r="C567" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D567">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="568" spans="1:4">
@@ -11790,10 +11790,10 @@
         <v>-1.63119564389893</v>
       </c>
       <c r="C569" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D569">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="570" spans="1:4">
@@ -11804,10 +11804,10 @@
         <v>-1.870308325759753</v>
       </c>
       <c r="C570" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D570">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="571" spans="1:4">
@@ -11818,10 +11818,10 @@
         <v>-1.71799640221788</v>
       </c>
       <c r="C571" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D571">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="572" spans="1:4">
@@ -11832,10 +11832,10 @@
         <v>-1.624312730075343</v>
       </c>
       <c r="C572" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D572">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="573" spans="1:4">
@@ -11902,10 +11902,10 @@
         <v>-1.588096056750363</v>
       </c>
       <c r="C577" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D577">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="578" spans="1:4">
@@ -12000,10 +12000,10 @@
         <v>-1.669691757061843</v>
       </c>
       <c r="C584" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D584">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="585" spans="1:4">
@@ -12014,10 +12014,10 @@
         <v>-1.682106005773208</v>
       </c>
       <c r="C585" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D585">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="586" spans="1:4">
@@ -12028,10 +12028,10 @@
         <v>-1.736289664964156</v>
       </c>
       <c r="C586" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D586">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="587" spans="1:4">
@@ -12056,10 +12056,10 @@
         <v>-1.565161799317006</v>
       </c>
       <c r="C588" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D588">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="589" spans="1:4">
@@ -12084,10 +12084,10 @@
         <v>-1.993343097224401</v>
       </c>
       <c r="C590" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D590">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="591" spans="1:4">
@@ -12098,10 +12098,10 @@
         <v>-1.988740434599921</v>
       </c>
       <c r="C591" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D591">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="592" spans="1:4">
@@ -12126,10 +12126,10 @@
         <v>-1.663856119008546</v>
       </c>
       <c r="C593" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D593">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="594" spans="1:4">
@@ -12196,10 +12196,10 @@
         <v>-1.577538301693559</v>
       </c>
       <c r="C598" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D598">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="599" spans="1:4">
@@ -12266,10 +12266,10 @@
         <v>-1.678233491537891</v>
       </c>
       <c r="C603" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D603">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="604" spans="1:4">
@@ -12392,10 +12392,10 @@
         <v>-1.742698146370599</v>
       </c>
       <c r="C612" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D612">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="613" spans="1:4">
@@ -12448,10 +12448,10 @@
         <v>-1.916950956727843</v>
       </c>
       <c r="C616" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D616">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="617" spans="1:4">
@@ -12644,10 +12644,10 @@
         <v>-1.638301694188023</v>
       </c>
       <c r="C630" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D630">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="631" spans="1:4">
@@ -12840,10 +12840,10 @@
         <v>-1.97768026021477</v>
       </c>
       <c r="C644" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D644">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="645" spans="1:4">
@@ -12854,10 +12854,10 @@
         <v>-1.88593836241727</v>
       </c>
       <c r="C645" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D645">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="646" spans="1:4">
@@ -12938,10 +12938,10 @@
         <v>-1.819416168716228</v>
       </c>
       <c r="C651" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D651">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="652" spans="1:4">
@@ -12952,10 +12952,10 @@
         <v>-1.729059563252198</v>
       </c>
       <c r="C652" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D652">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="653" spans="1:4">
@@ -12980,10 +12980,10 @@
         <v>-1.583958234398283</v>
       </c>
       <c r="C654" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D654">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="655" spans="1:4">
@@ -13036,10 +13036,10 @@
         <v>-1.797732230517901</v>
       </c>
       <c r="C658" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D658">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="659" spans="1:4">
@@ -13050,10 +13050,10 @@
         <v>-1.759756635387994</v>
       </c>
       <c r="C659" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D659">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="660" spans="1:4">
@@ -13176,10 +13176,10 @@
         <v>-1.698074632038931</v>
       </c>
       <c r="C668" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D668">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="669" spans="1:4">
@@ -13204,10 +13204,10 @@
         <v>-1.665908662080204</v>
       </c>
       <c r="C670" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D670">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="671" spans="1:4">
@@ -13260,10 +13260,10 @@
         <v>-1.963536101179138</v>
       </c>
       <c r="C674" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D674">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="675" spans="1:4">
@@ -13274,10 +13274,10 @@
         <v>-1.947706386533959</v>
       </c>
       <c r="C675" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D675">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="676" spans="1:4">
@@ -13316,10 +13316,10 @@
         <v>-2.027892937841425</v>
       </c>
       <c r="C678" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D678">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="679" spans="1:4">
@@ -13330,10 +13330,10 @@
         <v>-2.045941303721229</v>
       </c>
       <c r="C679" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D679">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="680" spans="1:4">
@@ -13358,10 +13358,10 @@
         <v>-1.763831100537918</v>
       </c>
       <c r="C681" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D681">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="682" spans="1:4">
@@ -13400,10 +13400,10 @@
         <v>-1.938106452866861</v>
       </c>
       <c r="C684" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D684">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="685" spans="1:4">
@@ -13442,10 +13442,10 @@
         <v>-1.669063381747349</v>
       </c>
       <c r="C687" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D687">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="688" spans="1:4">
@@ -13512,10 +13512,10 @@
         <v>-1.876577504083892</v>
       </c>
       <c r="C692" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D692">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="693" spans="1:4">
@@ -13596,10 +13596,10 @@
         <v>-1.612580279820375</v>
       </c>
       <c r="C698" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D698">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="699" spans="1:4">
@@ -13624,10 +13624,10 @@
         <v>-1.770945211869742</v>
       </c>
       <c r="C700" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D700">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="701" spans="1:4">
@@ -13666,10 +13666,10 @@
         <v>-1.942334796667527</v>
       </c>
       <c r="C703" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D703">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="704" spans="1:4">
@@ -13680,10 +13680,10 @@
         <v>-1.813351179675784</v>
       </c>
       <c r="C704" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D704">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="705" spans="1:4">
@@ -13722,10 +13722,10 @@
         <v>-1.690075472623206</v>
       </c>
       <c r="C707" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D707">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="708" spans="1:4">
@@ -13750,10 +13750,10 @@
         <v>-1.802997913173723</v>
       </c>
       <c r="C709" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D709">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="710" spans="1:4">
@@ -13764,10 +13764,10 @@
         <v>-1.614678444172489</v>
       </c>
       <c r="C710" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D710">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="711" spans="1:4">
@@ -13820,10 +13820,10 @@
         <v>-2.036469615049466</v>
       </c>
       <c r="C714" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D714">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="715" spans="1:4">
@@ -13834,10 +13834,10 @@
         <v>-2.019278608236277</v>
       </c>
       <c r="C715" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D715">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="716" spans="1:4">
@@ -13946,10 +13946,10 @@
         <v>-1.575419580507796</v>
       </c>
       <c r="C723" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D723">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="724" spans="1:4">
@@ -13988,10 +13988,10 @@
         <v>-1.615002311645418</v>
       </c>
       <c r="C726" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D726">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="727" spans="1:4">
@@ -14030,10 +14030,10 @@
         <v>-1.847708314939652</v>
       </c>
       <c r="C729" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D729">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="730" spans="1:4">
@@ -14058,10 +14058,10 @@
         <v>-1.634615052927588</v>
       </c>
       <c r="C731" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D731">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="732" spans="1:4">
@@ -14156,10 +14156,10 @@
         <v>-1.544837115778711</v>
       </c>
       <c r="C738" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D738">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="739" spans="1:4">
@@ -14170,10 +14170,10 @@
         <v>-1.838795024660925</v>
       </c>
       <c r="C739" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D739">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="740" spans="1:4">
@@ -14324,10 +14324,10 @@
         <v>-1.831068630836528</v>
       </c>
       <c r="C750" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D750">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="751" spans="1:4">
@@ -14352,10 +14352,10 @@
         <v>-1.830620701973297</v>
       </c>
       <c r="C752" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D752">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="753" spans="1:4">
@@ -14394,10 +14394,10 @@
         <v>-2.058812573568705</v>
       </c>
       <c r="C755" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D755">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="756" spans="1:4">
@@ -14408,10 +14408,10 @@
         <v>-2.032931960280198</v>
       </c>
       <c r="C756" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D756">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="757" spans="1:4">
@@ -14520,10 +14520,10 @@
         <v>-1.579545991113843</v>
       </c>
       <c r="C764" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D764">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="765" spans="1:4">
@@ -14534,10 +14534,10 @@
         <v>-2.01854052756817</v>
       </c>
       <c r="C765" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D765">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="766" spans="1:4">
@@ -14590,10 +14590,10 @@
         <v>-2.073034250541492</v>
       </c>
       <c r="C769" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D769">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="770" spans="1:4">
@@ -14604,10 +14604,10 @@
         <v>-1.601258882286194</v>
       </c>
       <c r="C770" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D770">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="771" spans="1:4">
@@ -14632,10 +14632,10 @@
         <v>-1.766587505776208</v>
       </c>
       <c r="C772" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D772">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="773" spans="1:4">
@@ -14646,10 +14646,10 @@
         <v>-1.635892997046435</v>
       </c>
       <c r="C773" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D773">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="774" spans="1:4">
@@ -14660,10 +14660,10 @@
         <v>-1.82439936618413</v>
       </c>
       <c r="C774" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D774">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="775" spans="1:4">
@@ -14674,10 +14674,10 @@
         <v>-1.606152917310679</v>
       </c>
       <c r="C775" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D775">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="776" spans="1:4">
@@ -14716,10 +14716,10 @@
         <v>-1.813346875067343</v>
       </c>
       <c r="C778" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D778">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="779" spans="1:4">
@@ -14786,10 +14786,10 @@
         <v>-1.976627651611558</v>
       </c>
       <c r="C783" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D783">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="784" spans="1:4">
@@ -14800,10 +14800,10 @@
         <v>-1.680031187611942</v>
       </c>
       <c r="C784" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D784">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="785" spans="1:4">
@@ -14842,10 +14842,10 @@
         <v>-2.009504569759894</v>
       </c>
       <c r="C787" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D787">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="788" spans="1:4">
@@ -14856,10 +14856,10 @@
         <v>-1.736060909365292</v>
       </c>
       <c r="C788" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D788">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="789" spans="1:4">
@@ -14870,10 +14870,10 @@
         <v>-1.668701180912312</v>
       </c>
       <c r="C789" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D789">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="790" spans="1:4">
@@ -14940,10 +14940,10 @@
         <v>-1.808487517081057</v>
       </c>
       <c r="C794" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D794">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="795" spans="1:4">
@@ -15024,10 +15024,10 @@
         <v>-1.622471073769822</v>
       </c>
       <c r="C800" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D800">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="801" spans="1:4">
@@ -15038,10 +15038,10 @@
         <v>-1.618391440944486</v>
       </c>
       <c r="C801" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D801">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="802" spans="1:4">
@@ -15052,10 +15052,10 @@
         <v>-1.805596742094996</v>
       </c>
       <c r="C802" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D802">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="803" spans="1:4">
@@ -15066,10 +15066,10 @@
         <v>-2.008388509544614</v>
       </c>
       <c r="C803" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D803">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="804" spans="1:4">
@@ -15122,10 +15122,10 @@
         <v>-1.865381439208925</v>
       </c>
       <c r="C807" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D807">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="808" spans="1:4">
@@ -15178,10 +15178,10 @@
         <v>-1.592203826122518</v>
       </c>
       <c r="C811" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D811">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="812" spans="1:4">
@@ -15304,10 +15304,10 @@
         <v>-1.640636310782921</v>
       </c>
       <c r="C820" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D820">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="821" spans="1:4">
@@ -15318,10 +15318,10 @@
         <v>-1.736102090049736</v>
       </c>
       <c r="C821" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D821">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="822" spans="1:4">
@@ -15388,10 +15388,10 @@
         <v>-1.964191845579081</v>
       </c>
       <c r="C826" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D826">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="827" spans="1:4">
@@ -15444,10 +15444,10 @@
         <v>-1.756746184771272</v>
       </c>
       <c r="C830" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D830">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="831" spans="1:4">
@@ -15486,10 +15486,10 @@
         <v>-1.810847531662162</v>
       </c>
       <c r="C833" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D833">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="834" spans="1:4">
@@ -15598,10 +15598,10 @@
         <v>-1.99861657065968</v>
       </c>
       <c r="C841" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D841">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="842" spans="1:4">
@@ -15626,10 +15626,10 @@
         <v>-1.848057286517881</v>
       </c>
       <c r="C843" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D843">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="844" spans="1:4">
@@ -15640,10 +15640,10 @@
         <v>-1.76887969943253</v>
       </c>
       <c r="C844" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D844">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="845" spans="1:4">
@@ -15654,10 +15654,10 @@
         <v>-1.539415824304245</v>
       </c>
       <c r="C845" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D845">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="846" spans="1:4">
@@ -15780,10 +15780,10 @@
         <v>-2.048407762767778</v>
       </c>
       <c r="C854" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D854">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="855" spans="1:4">
@@ -15794,10 +15794,10 @@
         <v>-1.884088044769628</v>
       </c>
       <c r="C855" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D855">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="856" spans="1:4">
@@ -15892,10 +15892,10 @@
         <v>-1.824964591786535</v>
       </c>
       <c r="C862" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D862">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="863" spans="1:4">
@@ -15934,10 +15934,10 @@
         <v>-1.687720037822961</v>
       </c>
       <c r="C865" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D865">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="866" spans="1:4">
@@ -15948,10 +15948,10 @@
         <v>-1.881581188707223</v>
       </c>
       <c r="C866" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D866">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="867" spans="1:4">
@@ -15962,10 +15962,10 @@
         <v>-1.962835518054795</v>
       </c>
       <c r="C867" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D867">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="868" spans="1:4">
@@ -16060,10 +16060,10 @@
         <v>-1.726434025792006</v>
       </c>
       <c r="C874" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D874">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="875" spans="1:4">
@@ -16186,10 +16186,10 @@
         <v>-2.038137492296732</v>
       </c>
       <c r="C883" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D883">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="884" spans="1:4">
@@ -16228,10 +16228,10 @@
         <v>-2.015645777300202</v>
       </c>
       <c r="C886" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D886">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="887" spans="1:4">
@@ -16312,10 +16312,10 @@
         <v>-1.705635238918189</v>
       </c>
       <c r="C892" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D892">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="893" spans="1:4">
@@ -16326,10 +16326,10 @@
         <v>-1.937017806275409</v>
       </c>
       <c r="C893" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D893">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="894" spans="1:4">
@@ -16354,10 +16354,10 @@
         <v>-1.791948398151532</v>
       </c>
       <c r="C895" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D895">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="896" spans="1:4">
@@ -16382,10 +16382,10 @@
         <v>-1.624531554796152</v>
       </c>
       <c r="C897" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D897">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="898" spans="1:4">
@@ -16410,10 +16410,10 @@
         <v>-1.627142472032205</v>
       </c>
       <c r="C899" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D899">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="900" spans="1:4">
@@ -16438,10 +16438,10 @@
         <v>-1.9424291082879</v>
       </c>
       <c r="C901" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D901">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="902" spans="1:4">
@@ -16494,10 +16494,10 @@
         <v>-1.850135580687783</v>
       </c>
       <c r="C905" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D905">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="906" spans="1:4">
@@ -16508,10 +16508,10 @@
         <v>-1.750819363151055</v>
       </c>
       <c r="C906" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D906">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="907" spans="1:4">
@@ -16536,10 +16536,10 @@
         <v>-2.025167538696064</v>
       </c>
       <c r="C908" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D908">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="909" spans="1:4">
@@ -16648,10 +16648,10 @@
         <v>-1.680274453739573</v>
       </c>
       <c r="C916" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D916">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="917" spans="1:4">
@@ -16704,10 +16704,10 @@
         <v>-1.609944047695099</v>
       </c>
       <c r="C920" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D920">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="921" spans="1:4">
@@ -16718,10 +16718,10 @@
         <v>-1.842977720159522</v>
       </c>
       <c r="C921" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D921">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="922" spans="1:4">
@@ -16732,10 +16732,10 @@
         <v>-1.608504422942484</v>
       </c>
       <c r="C922" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D922">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="923" spans="1:4">
@@ -16746,10 +16746,10 @@
         <v>-2.063506597623396</v>
       </c>
       <c r="C923" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D923">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="924" spans="1:4">
@@ -16774,10 +16774,10 @@
         <v>-1.980217840584712</v>
       </c>
       <c r="C925" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D925">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="926" spans="1:4">
@@ -16788,10 +16788,10 @@
         <v>-1.851803483795998</v>
       </c>
       <c r="C926" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D926">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="927" spans="1:4">
@@ -16830,10 +16830,10 @@
         <v>-1.841275933161683</v>
       </c>
       <c r="C929" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D929">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="930" spans="1:4">
@@ -16956,10 +16956,10 @@
         <v>-1.616789493507204</v>
       </c>
       <c r="C938" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D938">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="939" spans="1:4">
@@ -17110,10 +17110,10 @@
         <v>-1.701176798524233</v>
       </c>
       <c r="C949" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D949">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="950" spans="1:4">
@@ -17222,10 +17222,10 @@
         <v>-2.061957675067921</v>
       </c>
       <c r="C957" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D957">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="958" spans="1:4">
@@ -17264,10 +17264,10 @@
         <v>-1.720127566080207</v>
       </c>
       <c r="C960" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D960">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="961" spans="1:4">
@@ -17278,10 +17278,10 @@
         <v>-1.948113769593824</v>
       </c>
       <c r="C961" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D961">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="962" spans="1:4">
@@ -17292,10 +17292,10 @@
         <v>-1.736577288035094</v>
       </c>
       <c r="C962" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D962">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="963" spans="1:4">
@@ -17334,10 +17334,10 @@
         <v>-1.912948296332935</v>
       </c>
       <c r="C965" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D965">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="966" spans="1:4">
@@ -17362,10 +17362,10 @@
         <v>-1.98916973303219</v>
       </c>
       <c r="C967" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D967">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="968" spans="1:4">
@@ -17376,10 +17376,10 @@
         <v>-1.907570817951796</v>
       </c>
       <c r="C968" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D968">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="969" spans="1:4">
@@ -17390,10 +17390,10 @@
         <v>-1.927631441758175</v>
       </c>
       <c r="C969" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D969">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="970" spans="1:4">
@@ -17404,10 +17404,10 @@
         <v>-1.90675851012764</v>
       </c>
       <c r="C970" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D970">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="971" spans="1:4">
@@ -17432,10 +17432,10 @@
         <v>-2.059726466761841</v>
       </c>
       <c r="C972" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D972">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="973" spans="1:4">
@@ -17502,10 +17502,10 @@
         <v>-1.944206451009739</v>
       </c>
       <c r="C977" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D977">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="978" spans="1:4">
@@ -17558,10 +17558,10 @@
         <v>-2.042252566375168</v>
       </c>
       <c r="C981" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D981">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="982" spans="1:4">
@@ -17586,10 +17586,10 @@
         <v>-1.783573144474161</v>
       </c>
       <c r="C983" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D983">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="984" spans="1:4">
@@ -17600,10 +17600,10 @@
         <v>-1.802516181256211</v>
       </c>
       <c r="C984" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D984">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="985" spans="1:4">
@@ -17712,10 +17712,10 @@
         <v>-2.067104759846854</v>
       </c>
       <c r="C992" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D992">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="993" spans="1:4">
@@ -17950,10 +17950,10 @@
         <v>-1.603664676333083</v>
       </c>
       <c r="C1009" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1009">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1010" spans="1:4">
@@ -18020,10 +18020,10 @@
         <v>-1.904623452187863</v>
       </c>
       <c r="C1014" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1014">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1015" spans="1:4">
@@ -18048,10 +18048,10 @@
         <v>-1.841424287755265</v>
       </c>
       <c r="C1016" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1016">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1017" spans="1:4">
@@ -18076,10 +18076,10 @@
         <v>-1.78156744526516</v>
       </c>
       <c r="C1018" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1018">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1019" spans="1:4">
@@ -18132,10 +18132,10 @@
         <v>-1.653439518199863</v>
       </c>
       <c r="C1022" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1022">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1023" spans="1:4">
@@ -18174,10 +18174,10 @@
         <v>-1.983509544546633</v>
       </c>
       <c r="C1025" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1025">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1026" spans="1:4">
@@ -18216,10 +18216,10 @@
         <v>-1.772220305382958</v>
       </c>
       <c r="C1028" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1028">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1029" spans="1:4">
@@ -18300,10 +18300,10 @@
         <v>-1.894067942343709</v>
       </c>
       <c r="C1034" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1034">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1035" spans="1:4">
@@ -18314,10 +18314,10 @@
         <v>-1.683018900344064</v>
       </c>
       <c r="C1035" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1035">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1036" spans="1:4">
@@ -18356,10 +18356,10 @@
         <v>-1.964633513613677</v>
       </c>
       <c r="C1038" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1038">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1039" spans="1:4">
@@ -18454,10 +18454,10 @@
         <v>-1.966078405150602</v>
       </c>
       <c r="C1045" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1045">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1046" spans="1:4">
@@ -18468,10 +18468,10 @@
         <v>-1.892699790216795</v>
       </c>
       <c r="C1046" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1046">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1047" spans="1:4">
@@ -18482,10 +18482,10 @@
         <v>-1.860099751246449</v>
       </c>
       <c r="C1047" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1047">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1048" spans="1:4">
@@ -18510,10 +18510,10 @@
         <v>-1.765578027696311</v>
       </c>
       <c r="C1049" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1049">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1050" spans="1:4">
@@ -18552,10 +18552,10 @@
         <v>-1.582441033255557</v>
       </c>
       <c r="C1052" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1052">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1053" spans="1:4">
@@ -18608,10 +18608,10 @@
         <v>-1.986453923010784</v>
       </c>
       <c r="C1056" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1056">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1057" spans="1:4">
@@ -18622,10 +18622,10 @@
         <v>-1.921934044441021</v>
       </c>
       <c r="C1057" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1057">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1058" spans="1:4">
@@ -18636,10 +18636,10 @@
         <v>-1.819604886970607</v>
       </c>
       <c r="C1058" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1058">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1059" spans="1:4">
@@ -18664,10 +18664,10 @@
         <v>-2.035683559065263</v>
       </c>
       <c r="C1060" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1060">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1061" spans="1:4">
@@ -18678,10 +18678,10 @@
         <v>-1.910938019463805</v>
       </c>
       <c r="C1061" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1061">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1062" spans="1:4">
@@ -18790,10 +18790,10 @@
         <v>-1.597856547387218</v>
       </c>
       <c r="C1069" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1069">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1070" spans="1:4">
@@ -18804,10 +18804,10 @@
         <v>-1.678521280996529</v>
       </c>
       <c r="C1070" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1070">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1071" spans="1:4">
@@ -18818,10 +18818,10 @@
         <v>-1.87154452418418</v>
       </c>
       <c r="C1071" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1071">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1072" spans="1:4">
@@ -18902,10 +18902,10 @@
         <v>-1.806488927508342</v>
       </c>
       <c r="C1077" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1077">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1078" spans="1:4">
@@ -18930,10 +18930,10 @@
         <v>-1.968648244659407</v>
       </c>
       <c r="C1079" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1079">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1080" spans="1:4">
@@ -18986,10 +18986,10 @@
         <v>-1.75681929397007</v>
       </c>
       <c r="C1083" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1083">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1084" spans="1:4">
@@ -19000,10 +19000,10 @@
         <v>-1.650849873829626</v>
       </c>
       <c r="C1084" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1084">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1085" spans="1:4">
@@ -19014,10 +19014,10 @@
         <v>-1.800760935205537</v>
       </c>
       <c r="C1085" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1085">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1086" spans="1:4">
@@ -19042,10 +19042,10 @@
         <v>-2.019569707130731</v>
       </c>
       <c r="C1087" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1087">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1088" spans="1:4">
@@ -19070,10 +19070,10 @@
         <v>-1.708438108998364</v>
       </c>
       <c r="C1089" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1089">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1090" spans="1:4">
@@ -19098,10 +19098,10 @@
         <v>-1.921558420523686</v>
       </c>
       <c r="C1091" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1091">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1092" spans="1:4">
@@ -19112,10 +19112,10 @@
         <v>-1.846353509952079</v>
       </c>
       <c r="C1092" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1092">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1093" spans="1:4">
@@ -19196,10 +19196,10 @@
         <v>-1.729076499492968</v>
       </c>
       <c r="C1098" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1098">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1099" spans="1:4">
@@ -19210,10 +19210,10 @@
         <v>-1.929105531204137</v>
       </c>
       <c r="C1099" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1099">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1100" spans="1:4">
@@ -19266,10 +19266,10 @@
         <v>-1.700243813501948</v>
       </c>
       <c r="C1103" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1103">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1104" spans="1:4">
@@ -19280,10 +19280,10 @@
         <v>-2.025314874162799</v>
       </c>
       <c r="C1104" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1104">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1105" spans="1:4">
@@ -19294,10 +19294,10 @@
         <v>-2.029833613888238</v>
       </c>
       <c r="C1105" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1105">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1106" spans="1:4">
@@ -19308,10 +19308,10 @@
         <v>-1.711795196801549</v>
       </c>
       <c r="C1106" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1106">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1107" spans="1:4">
@@ -19322,10 +19322,10 @@
         <v>-2.021128639806872</v>
       </c>
       <c r="C1107" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1107">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1108" spans="1:4">
@@ -19336,10 +19336,10 @@
         <v>-1.926475122999585</v>
       </c>
       <c r="C1108" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1108">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1109" spans="1:4">
@@ -19364,10 +19364,10 @@
         <v>-1.791043706286734</v>
       </c>
       <c r="C1110" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1110">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1111" spans="1:4">
@@ -19392,10 +19392,10 @@
         <v>-1.8640452669006</v>
       </c>
       <c r="C1112" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1112">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1113" spans="1:4">
@@ -19434,10 +19434,10 @@
         <v>-1.847510047175685</v>
       </c>
       <c r="C1115" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1115">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1116" spans="1:4">
@@ -19490,10 +19490,10 @@
         <v>-2.043979785508063</v>
       </c>
       <c r="C1119" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1119">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1120" spans="1:4">
@@ -19504,10 +19504,10 @@
         <v>-2.03132852362196</v>
       </c>
       <c r="C1120" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1120">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1121" spans="1:4">
@@ -19532,10 +19532,10 @@
         <v>-1.938669832212365</v>
       </c>
       <c r="C1122" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1122">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1123" spans="1:4">
@@ -19560,10 +19560,10 @@
         <v>-1.858734042659404</v>
       </c>
       <c r="C1124" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1124">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1125" spans="1:4">
@@ -19574,10 +19574,10 @@
         <v>-1.833487320131246</v>
       </c>
       <c r="C1125" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1125">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1126" spans="1:4">
@@ -19602,10 +19602,10 @@
         <v>-1.925724155393419</v>
       </c>
       <c r="C1127" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1127">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1128" spans="1:4">
@@ -19644,10 +19644,10 @@
         <v>-2.053008820499635</v>
       </c>
       <c r="C1130" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1130">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1131" spans="1:4">
@@ -19714,10 +19714,10 @@
         <v>-1.825155033216223</v>
       </c>
       <c r="C1135" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1135">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1136" spans="1:4">
@@ -19728,10 +19728,10 @@
         <v>-1.757559010204631</v>
       </c>
       <c r="C1136" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1136">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1137" spans="1:4">
@@ -19784,10 +19784,10 @@
         <v>-1.783277719142261</v>
       </c>
       <c r="C1140" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1140">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1141" spans="1:4">
@@ -19840,10 +19840,10 @@
         <v>-1.893516161928264</v>
       </c>
       <c r="C1144" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1144">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1145" spans="1:4">
@@ -19868,10 +19868,10 @@
         <v>-1.666784917361886</v>
       </c>
       <c r="C1146" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1146">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1147" spans="1:4">
@@ -19896,10 +19896,10 @@
         <v>-1.953075282573184</v>
       </c>
       <c r="C1148" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D1148">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>